<commit_message>
working on v2 stuff
</commit_message>
<xml_diff>
--- a/intermediateTables/鱼单价工具.xlsx
+++ b/intermediateTables/鱼单价工具.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5280" yWindow="765" windowWidth="41685" windowHeight="20190" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5430" yWindow="225" windowWidth="35295" windowHeight="20580" tabRatio="600" firstSheet="1" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="配置任务list" sheetId="1" state="visible" r:id="rId1"/>
@@ -905,7 +905,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" saveData="0" refreshOnLoad="1" refreshedBy="宋甫" refreshedDate="45772.49022199074" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="12">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" saveData="0" refreshOnLoad="1" refreshedBy="宋甫" refreshedDate="45784.75822685185" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="12">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:O13" sheet="切到多套"/>
   </cacheSource>
@@ -3521,10 +3521,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14" defaultRowHeight="12.75"/>
@@ -3569,238 +3569,238 @@
     <row r="2">
       <c r="A2" s="51" t="inlineStr">
         <is>
-          <t>Tench</t>
+          <t>Alewife</t>
         </is>
       </c>
       <c r="B2" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C2" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="51" t="n">
-        <v>540</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="51" t="inlineStr">
         <is>
-          <t>Tench</t>
+          <t>Alewife</t>
         </is>
       </c>
       <c r="B3" s="51" t="inlineStr">
         <is>
-          <t>_Trophy</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C3" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="51" t="n">
-        <v>270</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="51" t="inlineStr">
         <is>
-          <t>Tench</t>
+          <t>Common_Shiner</t>
         </is>
       </c>
       <c r="B4" s="51" t="inlineStr">
         <is>
-          <t>_Unique</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C4" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="51" t="n">
-        <v>135</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="51" t="inlineStr">
         <is>
-          <t>Tench</t>
+          <t>Common_Shiner</t>
         </is>
       </c>
       <c r="B5" s="51" t="inlineStr">
         <is>
-          <t>_Apex</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C5" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="51" t="n">
-        <v>54</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="51" t="inlineStr">
         <is>
-          <t>Golden_Bream</t>
+          <t>Green_Sunfish</t>
         </is>
       </c>
       <c r="B6" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C6" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="51" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E6" s="51" t="n">
-        <v>540</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="51" t="inlineStr">
         <is>
-          <t>Golden_Bream</t>
+          <t>Green_Sunfish</t>
         </is>
       </c>
       <c r="B7" s="51" t="inlineStr">
         <is>
-          <t>_Trophy</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C7" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="51" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="51" t="n">
-        <v>270</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="51" t="inlineStr">
         <is>
-          <t>Golden_Bream</t>
+          <t>Pumpkinseed_Sunfish</t>
         </is>
       </c>
       <c r="B8" s="51" t="inlineStr">
         <is>
-          <t>_Unique</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C8" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8" s="51" t="n">
-        <v>135</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="51" t="inlineStr">
         <is>
-          <t>Golden_Bream</t>
+          <t>Pumpkinseed_Sunfish</t>
         </is>
       </c>
       <c r="B9" s="51" t="inlineStr">
         <is>
-          <t>_Apex</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C9" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="51" t="n">
-        <v>54</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="51" t="inlineStr">
         <is>
-          <t>Green_Sunfish</t>
+          <t>Bluegill_Sunfish</t>
         </is>
       </c>
       <c r="B10" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C10" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="51" t="n">
-        <v>685</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="51" t="inlineStr">
         <is>
-          <t>Green_Sunfish</t>
+          <t>Bluegill_Sunfish</t>
         </is>
       </c>
       <c r="B11" s="51" t="inlineStr">
         <is>
-          <t>_Trophy</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C11" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="51" t="n">
-        <v>342</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="51" t="inlineStr">
         <is>
-          <t>Green_Sunfish</t>
+          <t>Bluegill_Sunfish</t>
         </is>
       </c>
       <c r="B12" s="51" t="inlineStr">
         <is>
-          <t>_Unique</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C12" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="51" t="n">
-        <v>171</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="51" t="inlineStr">
         <is>
-          <t>Black_Crappie</t>
+          <t>Redear_Sunfish</t>
         </is>
       </c>
       <c r="B13" s="51" t="inlineStr">
@@ -3815,13 +3815,13 @@
         <v>2</v>
       </c>
       <c r="E13" s="51" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="51" t="inlineStr">
         <is>
-          <t>Black_Crappie</t>
+          <t>Redear_Sunfish</t>
         </is>
       </c>
       <c r="B14" s="51" t="inlineStr">
@@ -3836,18 +3836,18 @@
         <v>2</v>
       </c>
       <c r="E14" s="51" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="51" t="inlineStr">
         <is>
-          <t>White_Crappie</t>
+          <t>Redear_Sunfish</t>
         </is>
       </c>
       <c r="B15" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C15" s="51" t="n">
@@ -3857,207 +3857,207 @@
         <v>2</v>
       </c>
       <c r="E15" s="51" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="51" t="inlineStr">
         <is>
-          <t>White_Crappie</t>
+          <t>Yaqui_Sucker</t>
         </is>
       </c>
       <c r="B16" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C16" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" s="51" t="n">
-        <v>500</v>
+        <v>363</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="51" t="inlineStr">
         <is>
-          <t>Redspotted_Sunfish</t>
+          <t>Yaqui_Sucker</t>
         </is>
       </c>
       <c r="B17" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C17" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="51" t="n">
-        <v>500</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="51" t="inlineStr">
         <is>
-          <t>Redspotted_Sunfish</t>
+          <t>Yaqui_Sucker</t>
         </is>
       </c>
       <c r="B18" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C18" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="51" t="n">
-        <v>500</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="51" t="inlineStr">
         <is>
-          <t>Largemouth_Bass</t>
+          <t>Yaqui_Sucker</t>
         </is>
       </c>
       <c r="B19" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Unique</t>
         </is>
       </c>
       <c r="C19" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="51" t="n">
-        <v>500</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="51" t="inlineStr">
         <is>
-          <t>Largemouth_Bass</t>
+          <t>Buffalofish</t>
         </is>
       </c>
       <c r="B20" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C20" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="51" t="n">
-        <v>500</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="51" t="inlineStr">
         <is>
-          <t>Channel_Catfish</t>
+          <t>Buffalofish</t>
         </is>
       </c>
       <c r="B21" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C21" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" s="51" t="n">
-        <v>500</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="51" t="inlineStr">
         <is>
-          <t>Channel_Catfish</t>
+          <t>Buffalofish</t>
         </is>
       </c>
       <c r="B22" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C22" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" s="51" t="n">
-        <v>500</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="51" t="inlineStr">
         <is>
-          <t>Pumpkinseed_Sunfish</t>
+          <t>Buffalofish</t>
         </is>
       </c>
       <c r="B23" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Unique</t>
         </is>
       </c>
       <c r="C23" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E23" s="51" t="n">
-        <v>500</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="51" t="inlineStr">
         <is>
-          <t>Pumpkinseed_Sunfish</t>
+          <t>Bigmouth_Buffalo</t>
         </is>
       </c>
       <c r="B24" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C24" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E24" s="51" t="n">
-        <v>500</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="51" t="inlineStr">
         <is>
-          <t>Buffalofish</t>
+          <t>Bigmouth_Buffalo</t>
         </is>
       </c>
       <c r="B25" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C25" s="51" t="n">
@@ -4067,18 +4067,18 @@
         <v>3</v>
       </c>
       <c r="E25" s="51" t="n">
-        <v>500</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="51" t="inlineStr">
         <is>
-          <t>Buffalofish</t>
+          <t>Bigmouth_Buffalo</t>
         </is>
       </c>
       <c r="B26" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C26" s="51" t="n">
@@ -4088,265 +4088,265 @@
         <v>3</v>
       </c>
       <c r="E26" s="51" t="n">
-        <v>500</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="51" t="inlineStr">
         <is>
-          <t>Redear_Sunfish</t>
+          <t>Bigmouth_Buffalo</t>
         </is>
       </c>
       <c r="B27" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Unique</t>
         </is>
       </c>
       <c r="C27" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E27" s="51" t="n">
-        <v>500</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="51" t="inlineStr">
         <is>
-          <t>Redear_Sunfish</t>
+          <t>Tench</t>
         </is>
       </c>
       <c r="B28" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C28" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="51" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E28" s="51" t="n">
-        <v>500</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="51" t="inlineStr">
         <is>
-          <t>Bluegill_Sunfish</t>
+          <t>Tench</t>
         </is>
       </c>
       <c r="B29" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C29" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="51" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E29" s="51" t="n">
-        <v>500</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="51" t="inlineStr">
         <is>
-          <t>Bluegill_Sunfish</t>
+          <t>Tench</t>
         </is>
       </c>
       <c r="B30" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C30" s="51" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="51" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E30" s="51" t="n">
-        <v>500</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="51" t="inlineStr">
         <is>
-          <t>White_Channel_Catfish</t>
+          <t>Tench</t>
         </is>
       </c>
       <c r="B31" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Unique</t>
         </is>
       </c>
       <c r="C31" s="51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E31" s="51" t="n">
-        <v>540</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="51" t="inlineStr">
         <is>
-          <t>White_Channel_Catfish</t>
+          <t>Tench</t>
         </is>
       </c>
       <c r="B32" s="51" t="inlineStr">
         <is>
-          <t>_Trophy</t>
+          <t>_Apex</t>
         </is>
       </c>
       <c r="C32" s="51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32" s="51" t="n">
-        <v>270</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="51" t="inlineStr">
         <is>
-          <t>White_Channel_Catfish</t>
+          <t>Channel_Catfish</t>
         </is>
       </c>
       <c r="B33" s="51" t="inlineStr">
         <is>
-          <t>_Unique</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C33" s="51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E33" s="51" t="n">
-        <v>135</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="51" t="inlineStr">
         <is>
-          <t>White_Channel_Catfish</t>
+          <t>Channel_Catfish</t>
         </is>
       </c>
       <c r="B34" s="51" t="inlineStr">
         <is>
-          <t>_Apex</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C34" s="51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" s="51" t="n">
-        <v>54</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="51" t="inlineStr">
         <is>
-          <t>Striped_Bass</t>
+          <t>Channel_Catfish</t>
         </is>
       </c>
       <c r="B35" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C35" s="51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E35" s="51" t="n">
-        <v>540</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="51" t="inlineStr">
         <is>
-          <t>Striped_Bass</t>
+          <t>Channel_Catfish</t>
         </is>
       </c>
       <c r="B36" s="51" t="inlineStr">
         <is>
-          <t>_Trophy</t>
+          <t>_Unique</t>
         </is>
       </c>
       <c r="C36" s="51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" s="51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E36" s="51" t="n">
-        <v>270</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="51" t="inlineStr">
         <is>
-          <t>Striped_Bass</t>
+          <t>Channel_Catfish</t>
         </is>
       </c>
       <c r="B37" s="51" t="inlineStr">
         <is>
-          <t>_Unique</t>
+          <t>_Apex</t>
         </is>
       </c>
       <c r="C37" s="51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37" s="51" t="n">
-        <v>135</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="51" t="inlineStr">
         <is>
-          <t>Striped_Bass</t>
+          <t>Common_Shiner</t>
         </is>
       </c>
       <c r="B38" s="51" t="inlineStr">
         <is>
-          <t>_Apex</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C38" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D38" s="51" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E38" s="51" t="n">
-        <v>54</v>
+        <v>500</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="51" t="inlineStr">
         <is>
-          <t>Walleye</t>
+          <t>Common_Shiner</t>
         </is>
       </c>
       <c r="B39" s="51" t="inlineStr">
@@ -4358,28 +4358,28 @@
         <v>2</v>
       </c>
       <c r="D39" s="51" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E39" s="51" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="51" t="inlineStr">
         <is>
-          <t>Walleye</t>
+          <t>Bluegill_Sunfish</t>
         </is>
       </c>
       <c r="B40" s="51" t="inlineStr">
         <is>
-          <t>_Trophy</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C40" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D40" s="51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E40" s="51" t="n">
         <v>400</v>
@@ -4388,75 +4388,75 @@
     <row r="41">
       <c r="A41" s="51" t="inlineStr">
         <is>
-          <t>Walleye</t>
+          <t>Bluegill_Sunfish</t>
         </is>
       </c>
       <c r="B41" s="51" t="inlineStr">
         <is>
-          <t>_Unique</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C41" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E41" s="51" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="51" t="inlineStr">
         <is>
-          <t>Muskellunge</t>
+          <t>Bluegill_Sunfish</t>
         </is>
       </c>
       <c r="B42" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C42" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D42" s="51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E42" s="51" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="51" t="inlineStr">
         <is>
-          <t>Muskellunge</t>
+          <t>Redear_Sunfish</t>
         </is>
       </c>
       <c r="B43" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C43" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D43" s="51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" s="51" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="51" t="inlineStr">
         <is>
-          <t>Bowfin</t>
+          <t>Redear_Sunfish</t>
         </is>
       </c>
       <c r="B44" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Common</t>
         </is>
       </c>
       <c r="C44" s="51" t="n">
@@ -4466,18 +4466,18 @@
         <v>2</v>
       </c>
       <c r="E44" s="51" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="51" t="inlineStr">
         <is>
-          <t>Bowfin</t>
+          <t>Redear_Sunfish</t>
         </is>
       </c>
       <c r="B45" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C45" s="51" t="n">
@@ -4487,13 +4487,13 @@
         <v>2</v>
       </c>
       <c r="E45" s="51" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="51" t="inlineStr">
         <is>
-          <t>Channel_Catfish</t>
+          <t>American_Shad</t>
         </is>
       </c>
       <c r="B46" s="51" t="inlineStr">
@@ -4514,7 +4514,7 @@
     <row r="47">
       <c r="A47" s="51" t="inlineStr">
         <is>
-          <t>Channel_Catfish</t>
+          <t>American_Shad</t>
         </is>
       </c>
       <c r="B47" s="51" t="inlineStr">
@@ -4535,7 +4535,7 @@
     <row r="48">
       <c r="A48" s="51" t="inlineStr">
         <is>
-          <t>Largemouth_Bass</t>
+          <t>Rock_Bass</t>
         </is>
       </c>
       <c r="B48" s="51" t="inlineStr">
@@ -4556,7 +4556,7 @@
     <row r="49">
       <c r="A49" s="51" t="inlineStr">
         <is>
-          <t>Largemouth_Bass</t>
+          <t>Rock_Bass</t>
         </is>
       </c>
       <c r="B49" s="51" t="inlineStr">
@@ -4577,7 +4577,7 @@
     <row r="50">
       <c r="A50" s="51" t="inlineStr">
         <is>
-          <t>Black_Crappie</t>
+          <t>Bowfin</t>
         </is>
       </c>
       <c r="B50" s="51" t="inlineStr">
@@ -4598,7 +4598,7 @@
     <row r="51">
       <c r="A51" s="51" t="inlineStr">
         <is>
-          <t>Black_Crappie</t>
+          <t>Bowfin</t>
         </is>
       </c>
       <c r="B51" s="51" t="inlineStr">
@@ -4631,10 +4631,10 @@
         <v>2</v>
       </c>
       <c r="D52" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E52" s="51" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53">
@@ -4652,52 +4652,493 @@
         <v>2</v>
       </c>
       <c r="D53" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E53" s="51" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="51" t="inlineStr">
         <is>
-          <t>Rock_Bass</t>
+          <t>Yellow_Perch</t>
         </is>
       </c>
       <c r="B54" s="51" t="inlineStr">
         <is>
-          <t>_Young</t>
+          <t>_Trophy</t>
         </is>
       </c>
       <c r="C54" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D54" s="51" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E54" s="51" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="51" t="inlineStr">
         <is>
-          <t>Rock_Bass</t>
+          <t>Redfin_Pickerel</t>
         </is>
       </c>
       <c r="B55" s="51" t="inlineStr">
         <is>
-          <t>_Common</t>
+          <t>_Young</t>
         </is>
       </c>
       <c r="C55" s="51" t="n">
         <v>2</v>
       </c>
       <c r="D55" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" s="51" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="51" t="inlineStr">
+        <is>
+          <t>Redfin_Pickerel</t>
+        </is>
+      </c>
+      <c r="B56" s="51" t="inlineStr">
+        <is>
+          <t>_Common</t>
+        </is>
+      </c>
+      <c r="C56" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="E55" s="51" t="n">
-        <v>500</v>
+      <c r="D56" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" s="51" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="51" t="inlineStr">
+        <is>
+          <t>Redfin_Pickerel</t>
+        </is>
+      </c>
+      <c r="B57" s="51" t="inlineStr">
+        <is>
+          <t>_Trophy</t>
+        </is>
+      </c>
+      <c r="C57" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D57" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" s="51" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="51" t="inlineStr">
+        <is>
+          <t>Spotted_Bass</t>
+        </is>
+      </c>
+      <c r="B58" s="51" t="inlineStr">
+        <is>
+          <t>_Young</t>
+        </is>
+      </c>
+      <c r="C58" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D58" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E58" s="51" t="n">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="51" t="inlineStr">
+        <is>
+          <t>Spotted_Bass</t>
+        </is>
+      </c>
+      <c r="B59" s="51" t="inlineStr">
+        <is>
+          <t>_Common</t>
+        </is>
+      </c>
+      <c r="C59" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D59" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E59" s="51" t="n">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="51" t="inlineStr">
+        <is>
+          <t>Spotted_Bass</t>
+        </is>
+      </c>
+      <c r="B60" s="51" t="inlineStr">
+        <is>
+          <t>_Trophy</t>
+        </is>
+      </c>
+      <c r="C60" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D60" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" s="51" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="51" t="inlineStr">
+        <is>
+          <t>Spotted_Bass</t>
+        </is>
+      </c>
+      <c r="B61" s="51" t="inlineStr">
+        <is>
+          <t>_Unique</t>
+        </is>
+      </c>
+      <c r="C61" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D61" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E61" s="51" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="51" t="inlineStr">
+        <is>
+          <t>Largemouth_Bass</t>
+        </is>
+      </c>
+      <c r="B62" s="51" t="inlineStr">
+        <is>
+          <t>_Young</t>
+        </is>
+      </c>
+      <c r="C62" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D62" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E62" s="51" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="51" t="inlineStr">
+        <is>
+          <t>Largemouth_Bass</t>
+        </is>
+      </c>
+      <c r="B63" s="51" t="inlineStr">
+        <is>
+          <t>_Common</t>
+        </is>
+      </c>
+      <c r="C63" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D63" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E63" s="51" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="51" t="inlineStr">
+        <is>
+          <t>Largemouth_Bass</t>
+        </is>
+      </c>
+      <c r="B64" s="51" t="inlineStr">
+        <is>
+          <t>_Trophy</t>
+        </is>
+      </c>
+      <c r="C64" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D64" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E64" s="51" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="51" t="inlineStr">
+        <is>
+          <t>Largemouth_Bass</t>
+        </is>
+      </c>
+      <c r="B65" s="51" t="inlineStr">
+        <is>
+          <t>_Unique</t>
+        </is>
+      </c>
+      <c r="C65" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D65" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E65" s="51" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="51" t="inlineStr">
+        <is>
+          <t>Largemouth_Bass</t>
+        </is>
+      </c>
+      <c r="B66" s="51" t="inlineStr">
+        <is>
+          <t>_Apex</t>
+        </is>
+      </c>
+      <c r="C66" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D66" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E66" s="51" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="51" t="inlineStr">
+        <is>
+          <t>American_Eel</t>
+        </is>
+      </c>
+      <c r="B67" s="51" t="inlineStr">
+        <is>
+          <t>_Young</t>
+        </is>
+      </c>
+      <c r="C67" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D67" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E67" s="51" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="51" t="inlineStr">
+        <is>
+          <t>American_Eel</t>
+        </is>
+      </c>
+      <c r="B68" s="51" t="inlineStr">
+        <is>
+          <t>_Common</t>
+        </is>
+      </c>
+      <c r="C68" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D68" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E68" s="51" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="51" t="inlineStr">
+        <is>
+          <t>American_Eel</t>
+        </is>
+      </c>
+      <c r="B69" s="51" t="inlineStr">
+        <is>
+          <t>_Trophy</t>
+        </is>
+      </c>
+      <c r="C69" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D69" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E69" s="51" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="51" t="inlineStr">
+        <is>
+          <t>American_Eel</t>
+        </is>
+      </c>
+      <c r="B70" s="51" t="inlineStr">
+        <is>
+          <t>_Unique</t>
+        </is>
+      </c>
+      <c r="C70" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D70" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E70" s="51" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="51" t="inlineStr">
+        <is>
+          <t>American_Eel</t>
+        </is>
+      </c>
+      <c r="B71" s="51" t="inlineStr">
+        <is>
+          <t>_Apex</t>
+        </is>
+      </c>
+      <c r="C71" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D71" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E71" s="51" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="51" t="inlineStr">
+        <is>
+          <t>Walleye</t>
+        </is>
+      </c>
+      <c r="B72" s="51" t="inlineStr">
+        <is>
+          <t>_Young</t>
+        </is>
+      </c>
+      <c r="C72" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D72" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E72" s="51" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="51" t="inlineStr">
+        <is>
+          <t>Walleye</t>
+        </is>
+      </c>
+      <c r="B73" s="51" t="inlineStr">
+        <is>
+          <t>_Common</t>
+        </is>
+      </c>
+      <c r="C73" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D73" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E73" s="51" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="51" t="inlineStr">
+        <is>
+          <t>Walleye</t>
+        </is>
+      </c>
+      <c r="B74" s="51" t="inlineStr">
+        <is>
+          <t>_Trophy</t>
+        </is>
+      </c>
+      <c r="C74" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D74" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E74" s="51" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="51" t="inlineStr">
+        <is>
+          <t>Walleye</t>
+        </is>
+      </c>
+      <c r="B75" s="51" t="inlineStr">
+        <is>
+          <t>_Unique</t>
+        </is>
+      </c>
+      <c r="C75" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D75" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E75" s="51" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="51" t="inlineStr">
+        <is>
+          <t>Walleye</t>
+        </is>
+      </c>
+      <c r="B76" s="51" t="inlineStr">
+        <is>
+          <t>_Apex</t>
+        </is>
+      </c>
+      <c r="C76" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D76" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E76" s="51" t="n">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -9489,8 +9930,8 @@
   </sheetPr>
   <dimension ref="A1:V200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14" defaultRowHeight="12.75"/>

</xml_diff>